<commit_message>
feat: changed fecha pago
</commit_message>
<xml_diff>
--- a/helpers/templates/batchInfo/btnt.xlsx
+++ b/helpers/templates/batchInfo/btnt.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>ParentKey</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>InternalSerialNumber</t>
-  </si>
-  <si>
-    <t>WarehouseCode</t>
   </si>
   <si>
     <t>WhsCode</t>
@@ -499,7 +496,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -518,7 +515,6 @@
     <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -540,7 +536,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -560,32 +556,29 @@
       </c>
       <c r="M1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>18</v>
@@ -594,7 +587,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>10</v>
@@ -603,10 +596,7 @@
         <v>11</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>